<commit_message>
updates for may 13, 14, 15
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-05-14.xlsx
+++ b/EC/Train Runs and Enforcements 2016-05-14.xlsx
@@ -2217,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CK166"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U35" sqref="U35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15306,7 +15306,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="E3" sqref="E3:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>